<commit_message>
update: pdf and gitbook
</commit_message>
<xml_diff>
--- a/index/index.xlsx
+++ b/index/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmc\pipetbooks\basic\index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13BB987-8CE0-4F3F-B67A-FE930E3A3ABA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E9EECD-879C-4F78-B97B-4E5874F7B23B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECD2918D-62A0-4856-BE13-E9328C629C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="286">
   <si>
     <t>대각행렬</t>
   </si>
@@ -895,6 +895,15 @@
   </si>
   <si>
     <t>sigma matrix</t>
+  </si>
+  <si>
+    <t>$AES</t>
+  </si>
+  <si>
+    <t>$COVARIANCE</t>
+  </si>
+  <si>
+    <t>`-2LL</t>
   </si>
 </sst>
 </file>
@@ -1254,11 +1263,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820B1A01-E184-4A00-A964-5F70651C46A8}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3685,6 +3694,27 @@
         <v>282</v>
       </c>
     </row>
+    <row r="102" spans="2:7">
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="F104" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I58" xr:uid="{5F4D74AF-3B29-4796-93B0-9FAE611FB410}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I58">

</xml_diff>